<commit_message>
Finished Wireshark iperf data
</commit_message>
<xml_diff>
--- a/iperfData.xlsx
+++ b/iperfData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osavk\Downloads\WirelessProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBD6A59-F123-4849-8AE3-4A62391B236A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2119F21C-2905-4D67-96CD-84863CBF53F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11472" yWindow="-48" windowWidth="23136" windowHeight="12456" xr2:uid="{69D721DC-33AF-42D7-B2B0-8363F6587FE8}"/>
+    <workbookView xWindow="11424" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{69D721DC-33AF-42D7-B2B0-8363F6587FE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
   <si>
     <t>Sample #</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>No data came in</t>
+  </si>
+  <si>
+    <t>Only through to AP1</t>
   </si>
 </sst>
 </file>
@@ -135,9 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,7 +459,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,6 +558,18 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
+      <c r="C5">
+        <v>367362.70310305059</v>
+      </c>
+      <c r="D5" s="2">
+        <v>262480.65348450327</v>
+      </c>
+      <c r="E5">
+        <v>370932.87592106935</v>
+      </c>
+      <c r="F5">
+        <v>370932.87592106935</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -562,6 +578,18 @@
       <c r="B6" t="s">
         <v>3</v>
       </c>
+      <c r="C6" s="2">
+        <v>264452.7132816636</v>
+      </c>
+      <c r="D6">
+        <v>188182.18190097925</v>
+      </c>
+      <c r="E6">
+        <v>207114.8528878066</v>
+      </c>
+      <c r="F6">
+        <v>208737.56275615681</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -570,6 +598,18 @@
       <c r="B7" t="s">
         <v>3</v>
       </c>
+      <c r="C7">
+        <v>257750.8114219103</v>
+      </c>
+      <c r="D7">
+        <v>220238.16263582019</v>
+      </c>
+      <c r="E7">
+        <v>214053.29599775374</v>
+      </c>
+      <c r="F7">
+        <v>223781.14898661038</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -578,6 +618,18 @@
       <c r="B8" t="s">
         <v>3</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>134326.4909139977</v>
+      </c>
+      <c r="E8">
+        <v>155041.00609131181</v>
+      </c>
+      <c r="F8">
+        <v>142612.29698492322</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -586,6 +638,18 @@
       <c r="B9" t="s">
         <v>3</v>
       </c>
+      <c r="C9">
+        <v>12997.657506285314</v>
+      </c>
+      <c r="D9">
+        <v>135538.75341015623</v>
+      </c>
+      <c r="E9">
+        <v>376745.43860978761</v>
+      </c>
+      <c r="F9">
+        <v>298256.37825470453</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -835,8 +899,12 @@
       <c r="F21">
         <v>1785636.2167910852</v>
       </c>
+      <c r="G21" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Excel Files for graphs
</commit_message>
<xml_diff>
--- a/iperfData.xlsx
+++ b/iperfData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4291761cacc7c298/Documents/CMU/Spring 2021/18-452 Wireless Networking and Applications/WirelessProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="326" documentId="13_ncr:1_{2119F21C-2905-4D67-96CD-84863CBF53F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4F5E3DC1-A330-45F5-A267-451B8B8C6E14}"/>
+  <xr:revisionPtr revIDLastSave="333" documentId="13_ncr:1_{2119F21C-2905-4D67-96CD-84863CBF53F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D0414634-0B78-4A08-AC94-FF22AF5AD4E5}"/>
   <bookViews>
     <workbookView xWindow="11472" yWindow="-48" windowWidth="23136" windowHeight="12456" xr2:uid="{69D721DC-33AF-42D7-B2B0-8363F6587FE8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="53">
   <si>
     <t>Sample #</t>
   </si>
@@ -184,6 +184,15 @@
   </si>
   <si>
     <t>Access Point 3</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>ac</t>
   </si>
 </sst>
 </file>
@@ -1651,7 +1660,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4007,7 +4015,7 @@
   <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4249,11 +4257,11 @@
         <v>113</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O3:O11" si="2">SUM(N4,Q4,R4,S4)</f>
+        <f t="shared" ref="O4:O11" si="2">SUM(N4,Q4,R4,S4)</f>
         <v>484</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P3:P11" si="3">N4/O4*100</f>
+        <f t="shared" ref="P4:P11" si="3">N4/O4*100</f>
         <v>23.347107438016529</v>
       </c>
       <c r="Q4">
@@ -4697,6 +4705,13 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13">
+        <f>AVERAGE(K2:K3)</f>
+        <v>8.9355219582433385</v>
+      </c>
       <c r="T13" t="s">
         <v>38</v>
       </c>
@@ -4711,6 +4726,13 @@
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14">
+        <f>AVERAGE(K4:K7)</f>
+        <v>13.751857270808282</v>
+      </c>
       <c r="O14" t="s">
         <v>43</v>
       </c>
@@ -4738,6 +4760,13 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15">
+        <f>AVERAGE(K8:K11)</f>
+        <v>31.301196799918088</v>
+      </c>
       <c r="O15" t="s">
         <v>44</v>
       </c>

</xml_diff>